<commit_message>
manual bottom right done
</commit_message>
<xml_diff>
--- a/output_excel/obj_MINIPAKsro_ORDER2025079 (6)_filled_order_note.xlsx
+++ b/output_excel/obj_MINIPAKsro_ORDER2025079 (6)_filled_order_note.xlsx
@@ -15,7 +15,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <name val="Calibri"/>
       <color indexed="8"/>
@@ -116,6 +116,15 @@
       <color indexed="8"/>
       <sz val="11"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -155,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="78">
+  <borders count="82">
     <border>
       <left/>
       <right/>
@@ -1124,13 +1133,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="00000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="00000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" applyAlignment="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1593,15 +1646,25 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="68" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="78" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="78" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="79" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2773,10 +2836,7 @@
       </c>
       <c r="I4" s="149" t="inlineStr">
         <is>
-          <t>Embossingové údaje: WW = týždeň výroby sáčkov, YYYY = rok výroby sáčkov
-Embossingové údaje budú zahrnuté na logistických štítkoch a dodacích listoch.
-Sáčiky a hromadné obaly sa budú prepravovať na paletách EPAL.
-Archív: Áno, 20 ks mix</t>
+          <t>Embossingové údaje budú zahrnuté na logistických štítkoch a dodacích listoch.Sáčiky a hromadné obaly sa budú prepravovať na paletách EPAL.Archív: Áno, 20 ks mix</t>
         </is>
       </c>
       <c r="J4" s="136" t="n"/>
@@ -3374,154 +3434,150 @@
       <c r="K19" s="89" t="n"/>
       <c r="L19" s="171" t="n"/>
     </row>
-    <row r="20" ht="28.5" customHeight="1" s="129">
-      <c r="A20" s="92" t="n"/>
-      <c r="B20" s="93" t="n"/>
-      <c r="C20" s="94" t="n"/>
-      <c r="D20" s="94" t="n"/>
-      <c r="E20" s="94" t="n"/>
-      <c r="F20" s="94" t="n"/>
-      <c r="G20" s="95" t="n"/>
-      <c r="H20" s="95" t="n"/>
-      <c r="I20" s="96" t="n"/>
-      <c r="J20" s="96" t="n"/>
-      <c r="K20" s="97" t="n"/>
-      <c r="L20" s="98" t="n"/>
+    <row r="20" ht="25" customHeight="1" s="129">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" s="172" t="inlineStr"/>
+      <c r="C20" s="172" t="inlineStr"/>
+      <c r="D20" s="172" t="inlineStr"/>
+      <c r="E20" s="172" t="inlineStr"/>
+      <c r="F20" s="172" t="inlineStr"/>
+      <c r="G20" s="172" t="inlineStr"/>
+      <c r="H20" s="172" t="inlineStr"/>
+      <c r="I20" s="172" t="inlineStr"/>
+      <c r="J20" s="172" t="inlineStr"/>
+      <c r="K20" s="172" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
     </row>
-    <row r="21" ht="13.55" customHeight="1" s="129">
-      <c r="A21" s="99" t="n"/>
-      <c r="B21" s="100" t="n"/>
-      <c r="C21" s="101" t="n"/>
-      <c r="D21" s="101" t="n"/>
-      <c r="E21" s="101" t="n"/>
-      <c r="F21" s="101" t="n"/>
-      <c r="G21" s="102" t="n"/>
-      <c r="H21" s="103" t="n"/>
-      <c r="I21" s="172" t="inlineStr">
+    <row r="21" ht="25" customHeight="1" s="129">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" s="172" t="inlineStr"/>
+      <c r="C21" s="172" t="inlineStr"/>
+      <c r="D21" s="172" t="inlineStr"/>
+      <c r="E21" s="172" t="inlineStr"/>
+      <c r="F21" s="172" t="inlineStr"/>
+      <c r="G21" s="172" t="inlineStr"/>
+      <c r="H21" s="172" t="inlineStr"/>
+      <c r="I21" s="173" t="inlineStr">
         <is>
           <t>Expedícia objednávky</t>
         </is>
       </c>
-      <c r="J21" s="131" t="n"/>
-      <c r="K21" s="131" t="n"/>
-      <c r="L21" s="132" t="n"/>
+      <c r="J21" s="174" t="n"/>
+      <c r="K21" s="174" t="n"/>
+      <c r="L21" s="174" t="n"/>
     </row>
-    <row r="22" ht="28.5" customHeight="1" s="129">
-      <c r="A22" s="99" t="n"/>
-      <c r="B22" s="100" t="n"/>
-      <c r="C22" s="101" t="n"/>
-      <c r="D22" s="101" t="n"/>
-      <c r="E22" s="101" t="n"/>
-      <c r="F22" s="101" t="n"/>
-      <c r="G22" s="102" t="n"/>
-      <c r="H22" s="107" t="n"/>
-      <c r="I22" s="108" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Typ palty </t>
-        </is>
-      </c>
-      <c r="J22" s="109" t="inlineStr">
+    <row r="22" ht="25" customHeight="1" s="129">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" s="172" t="inlineStr"/>
+      <c r="C22" s="172" t="inlineStr"/>
+      <c r="D22" s="172" t="inlineStr"/>
+      <c r="E22" s="172" t="inlineStr"/>
+      <c r="F22" s="172" t="inlineStr"/>
+      <c r="G22" s="172" t="inlineStr"/>
+      <c r="H22" s="172" t="inlineStr"/>
+      <c r="I22" s="175" t="inlineStr">
+        <is>
+          <t>Typ palty</t>
+        </is>
+      </c>
+      <c r="J22" s="175" t="inlineStr">
         <is>
           <t>Rozmer</t>
         </is>
       </c>
-      <c r="K22" s="173" t="n"/>
-      <c r="L22" s="111" t="inlineStr">
+      <c r="K22" s="176" t="n"/>
+      <c r="L22" s="175" t="inlineStr">
         <is>
           <t>Váha</t>
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="112" t="n"/>
-      <c r="B23" s="113" t="n"/>
-      <c r="C23" s="114" t="n"/>
-      <c r="D23" s="114" t="n"/>
-      <c r="E23" s="114" t="n"/>
-      <c r="F23" s="114" t="n"/>
-      <c r="G23" s="102" t="n"/>
-      <c r="H23" s="107" t="n"/>
-      <c r="I23" s="115" t="n"/>
-      <c r="J23" s="116" t="n"/>
-      <c r="K23" s="174" t="n"/>
-      <c r="L23" s="118" t="n"/>
+    <row r="23" ht="25" customHeight="1" s="129">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" s="172" t="inlineStr"/>
+      <c r="C23" s="172" t="inlineStr"/>
+      <c r="D23" s="172" t="inlineStr"/>
+      <c r="E23" s="172" t="inlineStr"/>
+      <c r="F23" s="172" t="inlineStr"/>
+      <c r="G23" s="172" t="inlineStr"/>
+      <c r="H23" s="172" t="inlineStr"/>
+      <c r="I23" s="177" t="inlineStr"/>
+      <c r="J23" s="178" t="inlineStr"/>
+      <c r="K23" s="179" t="n"/>
+      <c r="L23" t="inlineStr"/>
     </row>
-    <row r="24">
-      <c r="A24" s="112" t="n"/>
-      <c r="B24" s="113" t="n"/>
-      <c r="C24" s="114" t="n"/>
-      <c r="D24" s="114" t="n"/>
-      <c r="E24" s="114" t="n"/>
-      <c r="F24" s="114" t="n"/>
-      <c r="G24" s="102" t="n"/>
-      <c r="H24" s="119" t="n"/>
-      <c r="I24" s="120" t="n"/>
-      <c r="J24" s="175" t="n"/>
-      <c r="K24" s="176" t="n"/>
-      <c r="L24" s="123" t="n"/>
+    <row r="24" ht="25" customHeight="1" s="129">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" s="172" t="inlineStr"/>
+      <c r="C24" s="172" t="inlineStr"/>
+      <c r="D24" s="172" t="inlineStr"/>
+      <c r="E24" s="172" t="inlineStr"/>
+      <c r="F24" s="172" t="inlineStr"/>
+      <c r="G24" s="172" t="inlineStr"/>
+      <c r="H24" s="172" t="inlineStr"/>
+      <c r="I24" s="177" t="inlineStr"/>
+      <c r="J24" s="179" t="n"/>
+      <c r="K24" s="179" t="n"/>
+      <c r="L24" t="inlineStr"/>
     </row>
-    <row r="25">
-      <c r="A25" s="112" t="n"/>
-      <c r="B25" s="113" t="n"/>
-      <c r="C25" s="114" t="n"/>
-      <c r="D25" s="114" t="n"/>
-      <c r="E25" s="114" t="n"/>
-      <c r="F25" s="114" t="n"/>
-      <c r="G25" s="102" t="n"/>
-      <c r="H25" s="119" t="n"/>
-      <c r="I25" s="120" t="n"/>
-      <c r="J25" s="175" t="n"/>
-      <c r="K25" s="176" t="n"/>
-      <c r="L25" s="123" t="n"/>
+    <row r="25" ht="25" customHeight="1" s="129">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" s="172" t="inlineStr"/>
+      <c r="C25" s="172" t="inlineStr"/>
+      <c r="D25" s="172" t="inlineStr"/>
+      <c r="E25" s="172" t="inlineStr"/>
+      <c r="F25" s="172" t="inlineStr"/>
+      <c r="G25" s="172" t="inlineStr"/>
+      <c r="H25" s="172" t="inlineStr"/>
+      <c r="I25" s="177" t="inlineStr"/>
+      <c r="J25" s="179" t="n"/>
+      <c r="K25" s="179" t="n"/>
+      <c r="L25" t="inlineStr"/>
     </row>
-    <row r="26">
-      <c r="A26" s="112" t="n"/>
-      <c r="B26" s="113" t="n"/>
-      <c r="C26" s="114" t="n"/>
-      <c r="D26" s="114" t="n"/>
-      <c r="E26" s="114" t="n"/>
-      <c r="F26" s="114" t="n"/>
-      <c r="G26" s="102" t="n"/>
-      <c r="H26" s="119" t="n"/>
-      <c r="I26" s="120" t="n"/>
-      <c r="J26" s="177" t="n"/>
-      <c r="K26" s="178" t="n"/>
-      <c r="L26" s="123" t="n"/>
+    <row r="26" ht="25" customHeight="1" s="129">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" s="172" t="inlineStr"/>
+      <c r="C26" s="172" t="inlineStr"/>
+      <c r="D26" s="172" t="inlineStr"/>
+      <c r="E26" s="172" t="inlineStr"/>
+      <c r="F26" s="172" t="inlineStr"/>
+      <c r="G26" s="172" t="inlineStr"/>
+      <c r="H26" s="172" t="inlineStr"/>
+      <c r="I26" s="177" t="inlineStr"/>
+      <c r="J26" s="179" t="n"/>
+      <c r="K26" s="179" t="n"/>
+      <c r="L26" t="inlineStr"/>
     </row>
-    <row r="27">
-      <c r="A27" s="124" t="n"/>
-      <c r="B27" s="125" t="n"/>
-      <c r="C27" s="124" t="n"/>
-      <c r="D27" s="124" t="n"/>
-      <c r="E27" s="124" t="n"/>
-      <c r="F27" s="124" t="n"/>
-      <c r="G27" s="124" t="n"/>
-      <c r="H27" s="124" t="n"/>
-      <c r="I27" s="124" t="n"/>
-      <c r="J27" s="126" t="n"/>
-      <c r="K27" s="127" t="n"/>
-      <c r="L27" s="125" t="n"/>
+    <row r="27" ht="25" customHeight="1" s="129">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" s="172" t="inlineStr"/>
+      <c r="C27" s="172" t="inlineStr"/>
+      <c r="D27" s="172" t="inlineStr"/>
+      <c r="E27" s="172" t="inlineStr"/>
+      <c r="F27" s="172" t="inlineStr"/>
+      <c r="G27" s="172" t="inlineStr"/>
+      <c r="H27" s="172" t="inlineStr"/>
+      <c r="I27" s="177" t="inlineStr"/>
+      <c r="J27" s="177" t="inlineStr"/>
+      <c r="K27" s="177" t="inlineStr"/>
+      <c r="L27" s="180" t="inlineStr"/>
     </row>
-    <row r="28">
-      <c r="A28" s="126" t="n"/>
-      <c r="B28" s="127" t="n"/>
-      <c r="C28" s="126" t="n"/>
-      <c r="D28" s="126" t="n"/>
-      <c r="E28" s="126" t="n"/>
-      <c r="F28" s="126" t="n"/>
-      <c r="G28" s="126" t="n"/>
-      <c r="H28" s="126" t="n"/>
-      <c r="I28" s="126" t="n"/>
-      <c r="J28" s="126" t="n"/>
-      <c r="K28" s="128" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="L28" s="127" t="n"/>
+    <row r="28" ht="25" customHeight="1" s="129">
+      <c r="A28" s="179" t="inlineStr"/>
+      <c r="B28" s="178" t="inlineStr"/>
+      <c r="C28" s="178" t="inlineStr"/>
+      <c r="D28" s="178" t="inlineStr"/>
+      <c r="E28" s="178" t="inlineStr"/>
+      <c r="F28" s="178" t="inlineStr"/>
+      <c r="G28" s="178" t="inlineStr"/>
+      <c r="H28" s="178" t="inlineStr"/>
+      <c r="I28" s="178" t="inlineStr"/>
+      <c r="J28" s="178" t="inlineStr"/>
+      <c r="K28" s="178" t="inlineStr"/>
+      <c r="L28" s="179" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="29">
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="E10:E11"/>
@@ -3534,7 +3590,9 @@
     <mergeCell ref="F2:H3"/>
     <mergeCell ref="I2:L3"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="J23:K26"/>
     <mergeCell ref="A10:A11"/>
+    <mergeCell ref="J22:K22"/>
     <mergeCell ref="F4:G7"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="K10:K11"/>
@@ -3542,6 +3600,7 @@
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I21:L21"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="I4:L9"/>
     <mergeCell ref="C4:E4"/>

</xml_diff>